<commit_message>
Changes before push to server, hopefully did not mess anything up too badly
</commit_message>
<xml_diff>
--- a/Anton Test/1065_Calculation/Final.xlsx
+++ b/Anton Test/1065_Calculation/Final.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="20">
   <si>
     <t>Final Emissions</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>DF</t>
   </si>
   <si>
     <t>FINAL Em.</t>
@@ -499,7 +496,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="J1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K1" s="2"/>
     </row>
@@ -525,22 +522,19 @@
       <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="J2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5">
         <v>757.343</v>
@@ -558,7 +552,7 @@
         <v>753.681</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" s="5">
         <v>15233.6930915101</v>
@@ -566,10 +560,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5">
         <v>8.334</v>
@@ -595,10 +589,10 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5">
         <v>0.198</v>
@@ -624,10 +618,10 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5">
         <v>0.317</v>
@@ -645,7 +639,7 @@
         <v>0.134</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="5">
         <v>6.38331247191475</v>
@@ -653,10 +647,10 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5">
         <v>0.271</v>
@@ -682,7 +676,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -692,7 +686,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="J10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -718,22 +712,19 @@
       <c r="G11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="J11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="5">
         <v>757.343</v>
@@ -751,7 +742,7 @@
         <v>753.681</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J12" s="5">
         <v>15233.6930915101</v>
@@ -759,10 +750,10 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="5">
         <v>8.334</v>
@@ -788,10 +779,10 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5">
         <v>0.198</v>
@@ -817,10 +808,10 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="5">
         <v>0.317</v>
@@ -838,7 +829,7 @@
         <v>0.134</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J15" s="5">
         <v>6.38331247191475</v>
@@ -846,10 +837,10 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="5">
         <v>0.271</v>
@@ -875,7 +866,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -885,7 +876,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="J19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K19" s="2"/>
     </row>
@@ -911,22 +902,19 @@
       <c r="G20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="J20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="5">
         <v>754.462</v>
@@ -944,7 +932,7 @@
         <v>750.814</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J21" s="5">
         <v>15175.7400158928</v>
@@ -952,10 +940,10 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="5">
         <v>8.347</v>
@@ -981,10 +969,10 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="5">
         <v>0.2</v>
@@ -1010,10 +998,10 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="5">
         <v>0.319</v>
@@ -1031,7 +1019,7 @@
         <v>0.135</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J24" s="5">
         <v>6.4206272155961</v>
@@ -1039,10 +1027,10 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="5">
         <v>0.27</v>

</xml_diff>